<commit_message>
adding docs, remove specific user tracking, update graphs
</commit_message>
<xml_diff>
--- a/seasonal-analysis.xlsx
+++ b/seasonal-analysis.xlsx
@@ -8,7 +8,11 @@
   </bookViews>
   <sheets>
     <sheet name="summaries.csv" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="summaries" localSheetId="1">Sheet1!$A$1:$D$11</definedName>
+  </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -18,8 +22,24 @@
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="summaries.csv" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:code:subject-user-mix-analyser:summaries.csv" comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
   <si>
     <t>season</t>
   </si>
@@ -95,6 +115,15 @@
   <si>
     <t xml:space="preserve">Number of anonymous IPs </t>
   </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t>returning</t>
+  </si>
+  <si>
+    <t>anon</t>
+  </si>
 </sst>
 </file>
 
@@ -102,8 +131,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.0%"/>
-    <numFmt numFmtId="168" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -154,10 +183,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -176,11 +209,11 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="21">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -189,6 +222,8 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
@@ -196,6 +231,8 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
@@ -330,31 +367,31 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.07413695529145E-5</c:v>
+                  <c:v>0.181734578381437</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>0.029538173009299</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.000228180262407302</c:v>
+                  <c:v>0.460239589275528</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.000521920668058455</c:v>
+                  <c:v>0.591231732776618</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0</c:v>
+                  <c:v>0.325269343780607</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.000487044613286577</c:v>
+                  <c:v>0.645528930450029</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0015922232464594</c:v>
+                  <c:v>0.685661610659515</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.0539239287433799</c:v>
+                  <c:v>0.303322099181512</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.0349608197709463</c:v>
+                  <c:v>0.160940325497287</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -423,31 +460,31 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.999929258630447</c:v>
+                  <c:v>0.818265421618562</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0</c:v>
+                  <c:v>0.970461826990701</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.999771819737593</c:v>
+                  <c:v>0.539760410724472</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.999478079331941</c:v>
+                  <c:v>0.408768267223382</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0</c:v>
+                  <c:v>0.674730656219393</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.999512955386713</c:v>
+                  <c:v>0.354471069549971</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.998407776753541</c:v>
+                  <c:v>0.314338389340484</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.94607607125662</c:v>
+                  <c:v>0.696677900818488</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.965039180229054</c:v>
+                  <c:v>0.839059674502712</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -463,11 +500,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2115076424"/>
-        <c:axId val="-2115972648"/>
+        <c:axId val="2037230600"/>
+        <c:axId val="2082850120"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2115076424"/>
+        <c:axId val="2037230600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -486,7 +523,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2115972648"/>
+        <c:crossAx val="2082850120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -494,7 +531,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2115972648"/>
+        <c:axId val="2082850120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -506,7 +543,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2115076424"/>
+        <c:crossAx val="2037230600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="0.05"/>
@@ -634,7 +671,7 @@
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>363321.0</c:v>
+                  <c:v>204651.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>302300.0</c:v>
@@ -676,11 +713,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2114404296"/>
-        <c:axId val="-2114658584"/>
+        <c:axId val="2082410376"/>
+        <c:axId val="2082413528"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2114404296"/>
+        <c:axId val="2082410376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -700,7 +737,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114658584"/>
+        <c:crossAx val="2082413528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -708,7 +745,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2114658584"/>
+        <c:axId val="2082413528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -720,7 +757,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2114404296"/>
+        <c:crossAx val="2082410376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -842,34 +879,34 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.124149168366266</c:v>
+                  <c:v>0.0587292512619044</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.30797221303341E-6</c:v>
+                  <c:v>0.00849818061528283</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>0.00170410743991669</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.16796164124849E-6</c:v>
+                  <c:v>0.0184917786303982</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.33485565922315E-5</c:v>
+                  <c:v>0.0264492449076798</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0</c:v>
+                  <c:v>0.0147733288255626</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.31739461501777E-5</c:v>
+                  <c:v>0.0174607482274455</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.52459822348009E-5</c:v>
+                  <c:v>0.0108717171918495</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.00153797563956442</c:v>
+                  <c:v>0.00865111297254988</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.00138006519618341</c:v>
+                  <c:v>0.00635305874794775</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -938,31 +975,31 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0467581872312272</c:v>
+                  <c:v>0.0382633145881575</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0576917008164388</c:v>
+                  <c:v>0.0559875933765221</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0401694239311303</c:v>
+                  <c:v>0.0216868132623733</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0447124858741233</c:v>
+                  <c:v>0.0182865895230357</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0454187555883753</c:v>
+                  <c:v>0.0306454267628127</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0270355722893947</c:v>
+                  <c:v>0.00958799800809934</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0158305595971273</c:v>
+                  <c:v>0.00498408838751254</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.0269832333191437</c:v>
+                  <c:v>0.0198700959861582</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.0380945582601661</c:v>
+                  <c:v>0.0331215647084017</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1028,7 +1065,7 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.875850831633734</c:v>
+                  <c:v>0.941270748738096</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.95323850479656</c:v>
@@ -1071,11 +1108,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2109544040"/>
-        <c:axId val="-2108110856"/>
+        <c:axId val="2082448856"/>
+        <c:axId val="2082451864"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2109544040"/>
+        <c:axId val="2082448856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1095,7 +1132,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2108110856"/>
+        <c:crossAx val="2082451864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1103,7 +1140,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2108110856"/>
+        <c:axId val="2082451864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1115,7 +1152,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2109544040"/>
+        <c:crossAx val="2082448856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="0.05"/>
@@ -1416,34 +1453,34 @@
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>45106.0</c:v>
+                  <c:v>12019.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45107.0</c:v>
+                  <c:v>14588.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45107.0</c:v>
+                  <c:v>14966.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>45109.0</c:v>
+                  <c:v>19000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45114.0</c:v>
+                  <c:v>24664.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>45114.0</c:v>
+                  <c:v>27985.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>45119.0</c:v>
+                  <c:v>34612.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>45138.0</c:v>
+                  <c:v>42794.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>45250.0</c:v>
+                  <c:v>43424.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>45308.0</c:v>
+                  <c:v>43691.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1638,7 +1675,7 @@
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>45106.0</c:v>
+                  <c:v>12019.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>14136.0</c:v>
@@ -1682,11 +1719,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2108760472"/>
-        <c:axId val="-2113458696"/>
+        <c:axId val="2037289352"/>
+        <c:axId val="2037292520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2108760472"/>
+        <c:axId val="2037289352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1706,7 +1743,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2113458696"/>
+        <c:crossAx val="2037292520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1714,7 +1751,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2113458696"/>
+        <c:axId val="2037292520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1732,7 +1769,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2108760472"/>
+        <c:crossAx val="2037289352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1883,6 +1920,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="summaries" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2209,8 +2250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="F61" sqref="F61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2271,45 +2312,45 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>45106</v>
+        <v>12019</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>318215</v>
+        <v>192632</v>
       </c>
       <c r="E2" s="2">
-        <f>B2/L2</f>
+        <f t="shared" ref="E2:E11" si="0">B2/L2</f>
         <v>1</v>
       </c>
       <c r="F2" s="3">
-        <f>C2/L2</f>
+        <f t="shared" ref="F2:F11" si="1">C2/L2</f>
         <v>0</v>
       </c>
       <c r="G2" s="3">
-        <f>B2/J2</f>
-        <v>0.12414916836626565</v>
+        <f t="shared" ref="G2:G11" si="2">B2/J2</f>
+        <v>5.8729251261904411E-2</v>
       </c>
       <c r="H2" s="3">
-        <f>C2/J2</f>
+        <f t="shared" ref="H2:H11" si="3">C2/J2</f>
         <v>0</v>
       </c>
       <c r="I2" s="3">
-        <f>D2/J2</f>
-        <v>0.87585083163373434</v>
+        <f t="shared" ref="I2:I11" si="4">D2/J2</f>
+        <v>0.94127074873809558</v>
       </c>
       <c r="J2" s="4">
-        <f>B2+C2+D2</f>
-        <v>363321</v>
+        <f t="shared" ref="J2:J11" si="5">B2+C2+D2</f>
+        <v>204651</v>
       </c>
       <c r="K2" s="4">
         <f>B2+C2</f>
-        <v>45106</v>
+        <v>12019</v>
       </c>
       <c r="L2" s="4">
         <f>B2</f>
-        <v>45106</v>
+        <v>12019</v>
       </c>
       <c r="M2" t="s">
         <v>2</v>
@@ -2320,44 +2361,44 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2569</v>
       </c>
       <c r="C3">
-        <v>14135</v>
+        <v>11567</v>
       </c>
       <c r="D3">
         <v>288164</v>
       </c>
       <c r="E3" s="2">
-        <f>B3/L3</f>
-        <v>7.0741369552914548E-5</v>
+        <f t="shared" si="0"/>
+        <v>0.18173457838143747</v>
       </c>
       <c r="F3" s="3">
-        <f>C3/L3</f>
-        <v>0.99992925863044713</v>
+        <f t="shared" si="1"/>
+        <v>0.81826542161856253</v>
       </c>
       <c r="G3" s="3">
-        <f>B3/J3</f>
-        <v>3.3079722130334106E-6</v>
+        <f t="shared" si="2"/>
+        <v>8.4981806152828309E-3</v>
       </c>
       <c r="H3" s="3">
-        <f>C3/J3</f>
-        <v>4.6758187231227259E-2</v>
+        <f t="shared" si="3"/>
+        <v>3.826331458815746E-2</v>
       </c>
       <c r="I3" s="3">
-        <f>D3/J3</f>
+        <f t="shared" si="4"/>
         <v>0.95323850479655969</v>
       </c>
       <c r="J3" s="4">
-        <f>B3+C3+D3</f>
+        <f t="shared" si="5"/>
         <v>302300</v>
       </c>
       <c r="K3" s="4">
-        <f>K2+B3</f>
-        <v>45107</v>
+        <f t="shared" ref="K3:K11" si="6">K2+B3</f>
+        <v>14588</v>
       </c>
       <c r="L3" s="4">
-        <f>B3+C3</f>
+        <f t="shared" ref="L3:L11" si="7">B3+C3</f>
         <v>14136</v>
       </c>
       <c r="M3" t="s">
@@ -2369,44 +2410,44 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>378</v>
       </c>
       <c r="C4">
-        <v>12797</v>
+        <v>12419</v>
       </c>
       <c r="D4">
         <v>209020</v>
       </c>
       <c r="E4" s="2">
-        <f>B4/L4</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2.9538173009299055E-2</v>
       </c>
       <c r="F4" s="3">
-        <f>C4/L4</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>0.97046182699070094</v>
       </c>
       <c r="G4" s="3">
-        <f>B4/J4</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1.704107439916688E-3</v>
       </c>
       <c r="H4" s="3">
-        <f>C4/J4</f>
-        <v>5.7691700816438776E-2</v>
+        <f t="shared" si="3"/>
+        <v>5.5987593376522087E-2</v>
       </c>
       <c r="I4" s="3">
-        <f>D4/J4</f>
+        <f t="shared" si="4"/>
         <v>0.94230829918356118</v>
       </c>
       <c r="J4" s="4">
-        <f>B4+C4+D4</f>
+        <f t="shared" si="5"/>
         <v>221817</v>
       </c>
       <c r="K4" s="4">
-        <f>K3+B4</f>
-        <v>45107</v>
+        <f t="shared" si="6"/>
+        <v>14966</v>
       </c>
       <c r="L4" s="4">
-        <f>B4+C4</f>
+        <f t="shared" si="7"/>
         <v>12797</v>
       </c>
       <c r="M4" t="s">
@@ -2418,44 +2459,44 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>4034</v>
       </c>
       <c r="C5">
-        <v>8763</v>
+        <v>4731</v>
       </c>
       <c r="D5">
         <v>209386</v>
       </c>
       <c r="E5" s="2">
-        <f>B5/L5</f>
-        <v>2.2818026240730178E-4</v>
+        <f t="shared" si="0"/>
+        <v>0.46023958927552766</v>
       </c>
       <c r="F5" s="3">
-        <f>C5/L5</f>
-        <v>0.99977181973759266</v>
+        <f t="shared" si="1"/>
+        <v>0.53976041072447234</v>
       </c>
       <c r="G5" s="3">
-        <f>B5/J5</f>
-        <v>9.1679616412484926E-6</v>
+        <f t="shared" si="2"/>
+        <v>1.849177863039821E-2</v>
       </c>
       <c r="H5" s="3">
-        <f>C5/J5</f>
-        <v>4.0169423931130273E-2</v>
+        <f t="shared" si="3"/>
+        <v>2.168681326237331E-2</v>
       </c>
       <c r="I5" s="3">
-        <f>D5/J5</f>
+        <f t="shared" si="4"/>
         <v>0.95982140810722849</v>
       </c>
       <c r="J5" s="4">
-        <f>B5+C5+D5</f>
+        <f t="shared" si="5"/>
         <v>218151</v>
       </c>
       <c r="K5" s="4">
-        <f>K4+B5</f>
-        <v>45109</v>
+        <f t="shared" si="6"/>
+        <v>19000</v>
       </c>
       <c r="L5" s="4">
-        <f>B5+C5</f>
+        <f t="shared" si="7"/>
         <v>8765</v>
       </c>
       <c r="M5" s="1" t="s">
@@ -2467,44 +2508,44 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>5664</v>
       </c>
       <c r="C6">
-        <v>9575</v>
+        <v>3916</v>
       </c>
       <c r="D6">
         <v>204566</v>
       </c>
       <c r="E6" s="2">
-        <f>B6/L6</f>
-        <v>5.2192066805845506E-4</v>
+        <f t="shared" si="0"/>
+        <v>0.591231732776618</v>
       </c>
       <c r="F6" s="3">
-        <f>C6/L6</f>
-        <v>0.99947807933194155</v>
+        <f t="shared" si="1"/>
+        <v>0.40876826722338205</v>
       </c>
       <c r="G6" s="3">
-        <f>B6/J6</f>
-        <v>2.3348556592231469E-5</v>
+        <f t="shared" si="2"/>
+        <v>2.6449244907679807E-2</v>
       </c>
       <c r="H6" s="3">
-        <f>C6/J6</f>
-        <v>4.4712485874123263E-2</v>
+        <f t="shared" si="3"/>
+        <v>1.8286589523035687E-2</v>
       </c>
       <c r="I6" s="3">
-        <f>D6/J6</f>
+        <f t="shared" si="4"/>
         <v>0.95526416556928451</v>
       </c>
       <c r="J6" s="4">
-        <f>B6+C6+D6</f>
+        <f t="shared" si="5"/>
         <v>214146</v>
       </c>
       <c r="K6" s="4">
-        <f>K5+B6</f>
-        <v>45114</v>
+        <f t="shared" si="6"/>
+        <v>24664</v>
       </c>
       <c r="L6" s="4">
-        <f>B6+C6</f>
+        <f t="shared" si="7"/>
         <v>9580</v>
       </c>
       <c r="M6" t="s">
@@ -2516,44 +2557,44 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>3321</v>
       </c>
       <c r="C7">
-        <v>10210</v>
+        <v>6889</v>
       </c>
       <c r="D7">
         <v>214587</v>
       </c>
       <c r="E7" s="2">
-        <f>B7/L7</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.32526934378060723</v>
       </c>
       <c r="F7" s="3">
-        <f>C7/L7</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>0.67473065621939277</v>
       </c>
       <c r="G7" s="3">
-        <f>B7/J7</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1.4773328825562619E-2</v>
       </c>
       <c r="H7" s="3">
-        <f>C7/J7</f>
-        <v>4.5418755588375291E-2</v>
+        <f t="shared" si="3"/>
+        <v>3.0645426762812671E-2</v>
       </c>
       <c r="I7" s="3">
-        <f>D7/J7</f>
+        <f t="shared" si="4"/>
         <v>0.95458124441162473</v>
       </c>
       <c r="J7" s="4">
-        <f>B7+C7+D7</f>
+        <f t="shared" si="5"/>
         <v>224797</v>
       </c>
       <c r="K7" s="4">
-        <f>K6+B7</f>
-        <v>45114</v>
+        <f t="shared" si="6"/>
+        <v>27985</v>
       </c>
       <c r="L7" s="4">
-        <f>B7+C7</f>
+        <f t="shared" si="7"/>
         <v>10210</v>
       </c>
       <c r="M7" t="s">
@@ -2565,44 +2606,44 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>5</v>
+        <v>6627</v>
       </c>
       <c r="C8">
-        <v>10261</v>
+        <v>3639</v>
       </c>
       <c r="D8">
         <v>369271</v>
       </c>
       <c r="E8" s="2">
-        <f>B8/L8</f>
-        <v>4.8704461328657707E-4</v>
+        <f t="shared" si="0"/>
+        <v>0.64552893045002924</v>
       </c>
       <c r="F8" s="3">
-        <f>C8/L8</f>
-        <v>0.99951295538671348</v>
+        <f t="shared" si="1"/>
+        <v>0.35447106954997076</v>
       </c>
       <c r="G8" s="3">
-        <f>B8/J8</f>
-        <v>1.3173946150177717E-5</v>
+        <f t="shared" si="2"/>
+        <v>1.7460748227445547E-2</v>
       </c>
       <c r="H8" s="3">
-        <f>C8/J8</f>
-        <v>2.703557228939471E-2</v>
+        <f t="shared" si="3"/>
+        <v>9.5879980080993427E-3</v>
       </c>
       <c r="I8" s="3">
-        <f>D8/J8</f>
+        <f t="shared" si="4"/>
         <v>0.97295125376445513</v>
       </c>
       <c r="J8" s="4">
-        <f>B8+C8+D8</f>
+        <f t="shared" si="5"/>
         <v>379537</v>
       </c>
       <c r="K8" s="4">
-        <f>K7+B8</f>
-        <v>45119</v>
+        <f t="shared" si="6"/>
+        <v>34612</v>
       </c>
       <c r="L8" s="4">
-        <f>B8+C8</f>
+        <f t="shared" si="7"/>
         <v>10266</v>
       </c>
       <c r="M8" t="s">
@@ -2614,44 +2655,44 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>19</v>
+        <v>8182</v>
       </c>
       <c r="C9">
-        <v>11914</v>
+        <v>3751</v>
       </c>
       <c r="D9">
         <v>740662</v>
       </c>
       <c r="E9" s="2">
-        <f>B9/L9</f>
-        <v>1.5922232464593983E-3</v>
+        <f t="shared" si="0"/>
+        <v>0.68566161065951559</v>
       </c>
       <c r="F9" s="3">
-        <f>C9/L9</f>
-        <v>0.99840777675354064</v>
+        <f t="shared" si="1"/>
+        <v>0.31433838934048436</v>
       </c>
       <c r="G9" s="3">
-        <f>B9/J9</f>
-        <v>2.5245982234800924E-5</v>
+        <f t="shared" si="2"/>
+        <v>1.0871717191849534E-2</v>
       </c>
       <c r="H9" s="3">
-        <f>C9/J9</f>
-        <v>1.5830559597127272E-2</v>
+        <f t="shared" si="3"/>
+        <v>4.9840883875125397E-3</v>
       </c>
       <c r="I9" s="3">
-        <f>D9/J9</f>
+        <f t="shared" si="4"/>
         <v>0.98414419442063794</v>
       </c>
       <c r="J9" s="4">
-        <f>B9+C9+D9</f>
+        <f t="shared" si="5"/>
         <v>752595</v>
       </c>
       <c r="K9" s="4">
-        <f>K8+B9</f>
-        <v>45138</v>
+        <f t="shared" si="6"/>
+        <v>42794</v>
       </c>
       <c r="L9" s="4">
-        <f>B9+C9</f>
+        <f t="shared" si="7"/>
         <v>11933</v>
       </c>
       <c r="M9" t="s">
@@ -2663,44 +2704,44 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>112</v>
+        <v>630</v>
       </c>
       <c r="C10">
-        <v>1965</v>
+        <v>1447</v>
       </c>
       <c r="D10">
         <v>70746</v>
       </c>
       <c r="E10" s="2">
-        <f>B10/L10</f>
-        <v>5.3923928743379874E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.30332209918151182</v>
       </c>
       <c r="F10" s="3">
-        <f>C10/L10</f>
-        <v>0.94607607125662008</v>
+        <f t="shared" si="1"/>
+        <v>0.69667790081848824</v>
       </c>
       <c r="G10" s="3">
-        <f>B10/J10</f>
-        <v>1.5379756395644234E-3</v>
+        <f t="shared" si="2"/>
+        <v>8.6511129725498816E-3</v>
       </c>
       <c r="H10" s="3">
-        <f>C10/J10</f>
-        <v>2.6983233319143676E-2</v>
+        <f t="shared" si="3"/>
+        <v>1.9870095986158218E-2</v>
       </c>
       <c r="I10" s="3">
-        <f>D10/J10</f>
+        <f t="shared" si="4"/>
         <v>0.97147879104129187</v>
       </c>
       <c r="J10" s="4">
-        <f>B10+C10+D10</f>
+        <f t="shared" si="5"/>
         <v>72823</v>
       </c>
       <c r="K10" s="4">
-        <f>K9+B10</f>
-        <v>45250</v>
+        <f t="shared" si="6"/>
+        <v>43424</v>
       </c>
       <c r="L10" s="4">
-        <f>B10+C10</f>
+        <f t="shared" si="7"/>
         <v>2077</v>
       </c>
       <c r="M10" t="s">
@@ -2712,44 +2753,44 @@
         <v>15</v>
       </c>
       <c r="B11">
-        <v>58</v>
+        <v>267</v>
       </c>
       <c r="C11">
-        <v>1601</v>
+        <v>1392</v>
       </c>
       <c r="D11">
         <v>40368</v>
       </c>
       <c r="E11" s="2">
-        <f>B11/L11</f>
-        <v>3.4960819770946353E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.16094032549728751</v>
       </c>
       <c r="F11" s="3">
-        <f>C11/L11</f>
-        <v>0.96503918022905366</v>
+        <f t="shared" si="1"/>
+        <v>0.83905967450271246</v>
       </c>
       <c r="G11" s="3">
-        <f>B11/J11</f>
-        <v>1.3800651961834059E-3</v>
+        <f t="shared" si="2"/>
+        <v>6.353058747947748E-3</v>
       </c>
       <c r="H11" s="3">
-        <f>C11/J11</f>
-        <v>3.8094558260166084E-2</v>
+        <f t="shared" si="3"/>
+        <v>3.3121564708401739E-2</v>
       </c>
       <c r="I11" s="3">
-        <f>D11/J11</f>
+        <f t="shared" si="4"/>
         <v>0.96052537654365056</v>
       </c>
       <c r="J11" s="4">
-        <f>B11+C11+D11</f>
+        <f t="shared" si="5"/>
         <v>42027</v>
       </c>
       <c r="K11" s="4">
-        <f>K10+B11</f>
-        <v>45308</v>
+        <f t="shared" si="6"/>
+        <v>43691</v>
       </c>
       <c r="L11" s="4">
-        <f>B11+C11</f>
+        <f t="shared" si="7"/>
         <v>1659</v>
       </c>
       <c r="M11" t="s">
@@ -2766,4 +2807,217 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="A2:D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>12019</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>192632</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2569</v>
+      </c>
+      <c r="C3">
+        <v>11567</v>
+      </c>
+      <c r="D3">
+        <v>288164</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>378</v>
+      </c>
+      <c r="C4">
+        <v>12419</v>
+      </c>
+      <c r="D4">
+        <v>209020</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4034</v>
+      </c>
+      <c r="C5">
+        <v>4731</v>
+      </c>
+      <c r="D5">
+        <v>209386</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>5664</v>
+      </c>
+      <c r="C6">
+        <v>3916</v>
+      </c>
+      <c r="D6">
+        <v>204566</v>
+      </c>
+      <c r="F6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>3321</v>
+      </c>
+      <c r="C7">
+        <v>6889</v>
+      </c>
+      <c r="D7">
+        <v>214587</v>
+      </c>
+      <c r="F7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>6627</v>
+      </c>
+      <c r="C8">
+        <v>3639</v>
+      </c>
+      <c r="D8">
+        <v>369271</v>
+      </c>
+      <c r="F8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>8182</v>
+      </c>
+      <c r="C9">
+        <v>3751</v>
+      </c>
+      <c r="D9">
+        <v>740662</v>
+      </c>
+      <c r="F9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>630</v>
+      </c>
+      <c r="C10">
+        <v>1447</v>
+      </c>
+      <c r="D10">
+        <v>70746</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>267</v>
+      </c>
+      <c r="C11">
+        <v>1392</v>
+      </c>
+      <c r="D11">
+        <v>40368</v>
+      </c>
+      <c r="F11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated data (ensuring users don't get set back to earlier seasons if they encounter old images later)
</commit_message>
<xml_diff>
--- a/seasonal-analysis.xlsx
+++ b/seasonal-analysis.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="16220" tabRatio="500"/>
+    <workbookView xWindow="2020" yWindow="160" windowWidth="25360" windowHeight="16220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="summaries.csv" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="summaries" localSheetId="1">Sheet1!$A$1:$D$11</definedName>
+    <definedName name="summaries" localSheetId="1">Sheet1!$A$1:$C$11</definedName>
+    <definedName name="summaries_1" localSheetId="1">Sheet1!$A$18:$D$28</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -25,6 +26,17 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="summaries.csv" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:code:subject-user-mix-analyser:summaries.csv" comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" name="summaries.csv1" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Macintosh HD:code:subject-user-mix-analyser:summaries.csv" comma="1">
       <textFields count="5">
         <textField/>
@@ -195,10 +207,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -233,7 +251,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="35">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -248,6 +266,9 @@
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
@@ -261,6 +282,9 @@
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
@@ -317,6 +341,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -399,31 +424,31 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.181734578381437</c:v>
+                  <c:v>0.624819773429454</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.029538173009299</c:v>
+                  <c:v>0.354959046306058</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.460239589275528</c:v>
+                  <c:v>0.487457790641582</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.591231732776618</c:v>
+                  <c:v>0.529907445779804</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.325269343780607</c:v>
+                  <c:v>0.528841245533435</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.645528930450029</c:v>
+                  <c:v>0.676348126332893</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.685661610659515</c:v>
+                  <c:v>0.726693494299128</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.303322099181512</c:v>
+                  <c:v>0.300824842309558</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.160940325497287</c:v>
+                  <c:v>0.170584689572031</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -492,31 +517,31 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.818265421618562</c:v>
+                  <c:v>0.375180226570546</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.970461826990701</c:v>
+                  <c:v>0.645040953693942</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.539760410724472</c:v>
+                  <c:v>0.512542209358418</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.408768267223382</c:v>
+                  <c:v>0.470092554220196</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.674730656219393</c:v>
+                  <c:v>0.471158754466565</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.354471069549971</c:v>
+                  <c:v>0.323651873667107</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.314338389340484</c:v>
+                  <c:v>0.273306505700872</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.696677900818488</c:v>
+                  <c:v>0.699175157690441</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.839059674502712</c:v>
+                  <c:v>0.829415310427969</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -532,11 +557,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2136900712"/>
-        <c:axId val="-2136777976"/>
+        <c:axId val="2092169032"/>
+        <c:axId val="2093668360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2136900712"/>
+        <c:axId val="2092169032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -555,7 +580,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2136777976"/>
+        <c:crossAx val="2093668360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -563,7 +588,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2136777976"/>
+        <c:axId val="2093668360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -575,7 +600,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2136900712"/>
+        <c:crossAx val="2092169032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="0.05"/>
@@ -583,6 +608,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -723,31 +749,31 @@
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>204651.0</c:v>
+                  <c:v>196590.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>302300.0</c:v>
+                  <c:v>297874.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>221817.0</c:v>
+                  <c:v>221351.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>218151.0</c:v>
+                  <c:v>217678.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>214146.0</c:v>
+                  <c:v>211805.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>224797.0</c:v>
+                  <c:v>224382.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>379537.0</c:v>
+                  <c:v>379118.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>752595.0</c:v>
+                  <c:v>752590.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>72823.0</c:v>
+                  <c:v>72807.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>42027.0</c:v>
@@ -765,11 +791,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2136102088"/>
-        <c:axId val="-2134249128"/>
+        <c:axId val="2092130168"/>
+        <c:axId val="2092127048"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2136102088"/>
+        <c:axId val="2092130168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -789,7 +815,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2134249128"/>
+        <c:crossAx val="2092127048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -797,7 +823,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2134249128"/>
+        <c:axId val="2092127048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -809,7 +835,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2136102088"/>
+        <c:crossAx val="2092130168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -861,6 +887,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -930,34 +957,34 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.0587292512619044</c:v>
+                  <c:v>0.0201332722925886</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.00849818061528283</c:v>
+                  <c:v>0.0203676722372547</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.00170410743991669</c:v>
+                  <c:v>0.0197740240613324</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0184917786303982</c:v>
+                  <c:v>0.0185687115831641</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0264492449076798</c:v>
+                  <c:v>0.01811099832393</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0147733288255626</c:v>
+                  <c:v>0.0230856307546951</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0174607482274455</c:v>
+                  <c:v>0.0175670899297844</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0108717171918495</c:v>
+                  <c:v>0.011517559361671</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.00865111297254988</c:v>
+                  <c:v>0.00851566470256981</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.00635305874794775</c:v>
+                  <c:v>0.0067337663882742</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1026,31 +1053,31 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0382633145881575</c:v>
+                  <c:v>0.0122300032899817</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0559875933765221</c:v>
+                  <c:v>0.0359338787717245</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0216868132623733</c:v>
+                  <c:v>0.019524251417231</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0182865895230357</c:v>
+                  <c:v>0.016066665092892</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0306454267628127</c:v>
+                  <c:v>0.0205676034619533</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.00958799800809934</c:v>
+                  <c:v>0.00840635369462806</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.00498408838751254</c:v>
+                  <c:v>0.0043317078356077</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.0198700959861582</c:v>
+                  <c:v>0.0197920529619405</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.0331215647084017</c:v>
+                  <c:v>0.0327408570680753</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1116,31 +1143,31 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.941270748738096</c:v>
+                  <c:v>0.979866727707411</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.95323850479656</c:v>
+                  <c:v>0.967402324472764</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.942308299183561</c:v>
+                  <c:v>0.944292097166943</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.959821408107228</c:v>
+                  <c:v>0.961907036999605</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.955264165569284</c:v>
+                  <c:v>0.965822336583178</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.954581244411625</c:v>
+                  <c:v>0.956346765783352</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.972951253764455</c:v>
+                  <c:v>0.974026556375588</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.984144194420638</c:v>
+                  <c:v>0.984150732802721</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.971478791041292</c:v>
+                  <c:v>0.97169228233549</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.960525376543651</c:v>
@@ -1159,11 +1186,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2131811144"/>
-        <c:axId val="-2131808136"/>
+        <c:axId val="2092092376"/>
+        <c:axId val="2092089352"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2131811144"/>
+        <c:axId val="2092092376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1183,7 +1210,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2131808136"/>
+        <c:crossAx val="2092089352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1191,7 +1218,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2131808136"/>
+        <c:axId val="2092089352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1203,7 +1230,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131811144"/>
+        <c:crossAx val="2092092376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="0.05"/>
@@ -1211,6 +1238,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1340,8 +1368,8 @@
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.0245398773006135"/>
-                  <c:y val="-0.0299251870324189"/>
+                  <c:x val="-0.0257668711656441"/>
+                  <c:y val="-0.0448877805486283"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -1400,7 +1428,7 @@
               <c:idx val="5"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.0196319018404908"/>
+                  <c:x val="-0.0331288343558282"/>
                   <c:y val="-0.0349127182044888"/>
                 </c:manualLayout>
               </c:layout>
@@ -1415,8 +1443,8 @@
               <c:idx val="6"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.0171779141104294"/>
-                  <c:y val="-0.0274314214463841"/>
+                  <c:x val="-0.0478527607361963"/>
+                  <c:y val="-0.0324189526184539"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -1524,31 +1552,31 @@
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>12019.0</c:v>
+                  <c:v>3958.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14588.0</c:v>
+                  <c:v>10025.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14966.0</c:v>
+                  <c:v>14402.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19000.0</c:v>
+                  <c:v>18444.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24664.0</c:v>
+                  <c:v>22280.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>27985.0</c:v>
+                  <c:v>27460.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>34612.0</c:v>
+                  <c:v>34120.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>42794.0</c:v>
+                  <c:v>42788.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43424.0</c:v>
+                  <c:v>43408.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>43691.0</c:v>
@@ -1598,8 +1626,8 @@
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.00613496932515337"/>
-                  <c:y val="0.027431421446384"/>
+                  <c:x val="-0.0220859861842423"/>
+                  <c:y val="0.0349127182044888"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -1613,8 +1641,8 @@
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.00245398773006135"/>
-                  <c:y val="-0.0324189526184539"/>
+                  <c:x val="-0.0196319018404908"/>
+                  <c:y val="0.0399002493765586"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -1628,8 +1656,8 @@
               <c:idx val="2"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.0147239263803681"/>
-                  <c:y val="-0.0249376558603491"/>
+                  <c:x val="-0.026993961644365"/>
+                  <c:y val="0.0349127182044888"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -1714,6 +1742,21 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
             </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0220858895705523"/>
+                  <c:y val="-0.029925187032419"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -1767,31 +1810,31 @@
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>12019.0</c:v>
+                  <c:v>3958.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14136.0</c:v>
+                  <c:v>9710.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12797.0</c:v>
+                  <c:v>12331.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8765.0</c:v>
+                  <c:v>8292.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9580.0</c:v>
+                  <c:v>7239.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10210.0</c:v>
+                  <c:v>9795.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10266.0</c:v>
+                  <c:v>9847.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11933.0</c:v>
+                  <c:v>11928.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2077.0</c:v>
+                  <c:v>2061.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1659.0</c:v>
@@ -1811,11 +1854,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2134794472"/>
-        <c:axId val="-2138632440"/>
+        <c:axId val="2093709048"/>
+        <c:axId val="2093712104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2134794472"/>
+        <c:axId val="2093709048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1835,7 +1878,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2138632440"/>
+        <c:crossAx val="2093712104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1843,7 +1886,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2138632440"/>
+        <c:axId val="2093712104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1861,13 +1904,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2134794472"/>
+        <c:crossAx val="2093709048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
@@ -1926,6 +1969,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2005,34 +2049,34 @@
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>12019.0</c:v>
+                  <c:v>3958.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2569.0</c:v>
+                  <c:v>6067.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>378.0</c:v>
+                  <c:v>4377.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4034.0</c:v>
+                  <c:v>4042.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5664.0</c:v>
+                  <c:v>3836.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3321.0</c:v>
+                  <c:v>5180.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6627.0</c:v>
+                  <c:v>6660.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8182.0</c:v>
+                  <c:v>8668.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>630.0</c:v>
+                  <c:v>620.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>267.0</c:v>
+                  <c:v>283.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2101,31 +2145,31 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11567.0</c:v>
+                  <c:v>3643.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12419.0</c:v>
+                  <c:v>7954.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4731.0</c:v>
+                  <c:v>4250.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3916.0</c:v>
+                  <c:v>3403.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6889.0</c:v>
+                  <c:v>4615.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3639.0</c:v>
+                  <c:v>3187.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3751.0</c:v>
+                  <c:v>3260.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1447.0</c:v>
+                  <c:v>1441.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1392.0</c:v>
+                  <c:v>1376.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2141,11 +2185,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2135578632"/>
-        <c:axId val="-2133665432"/>
+        <c:axId val="2092038216"/>
+        <c:axId val="2092035192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2135578632"/>
+        <c:axId val="2092038216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2164,7 +2208,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133665432"/>
+        <c:crossAx val="2092035192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2172,7 +2216,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2133665432"/>
+        <c:axId val="2092035192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2184,13 +2228,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135578632"/>
+        <c:crossAx val="2092038216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2240,6 +2285,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2309,34 +2355,34 @@
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>12019.0</c:v>
+                  <c:v>3958.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2569.0</c:v>
+                  <c:v>6067.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>378.0</c:v>
+                  <c:v>4377.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4034.0</c:v>
+                  <c:v>4042.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5664.0</c:v>
+                  <c:v>3836.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3321.0</c:v>
+                  <c:v>5180.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6627.0</c:v>
+                  <c:v>6660.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8182.0</c:v>
+                  <c:v>8668.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>630.0</c:v>
+                  <c:v>620.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>267.0</c:v>
+                  <c:v>283.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2405,31 +2451,31 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11567.0</c:v>
+                  <c:v>3643.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12419.0</c:v>
+                  <c:v>7954.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4731.0</c:v>
+                  <c:v>4250.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3916.0</c:v>
+                  <c:v>3403.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6889.0</c:v>
+                  <c:v>4615.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3639.0</c:v>
+                  <c:v>3187.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3751.0</c:v>
+                  <c:v>3260.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1447.0</c:v>
+                  <c:v>1441.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1392.0</c:v>
+                  <c:v>1376.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2538,11 +2584,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2134940344"/>
-        <c:axId val="-2133073176"/>
+        <c:axId val="2091999784"/>
+        <c:axId val="2091996648"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2134940344"/>
+        <c:axId val="2091999784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2562,7 +2608,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133073176"/>
+        <c:crossAx val="2091996648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2570,7 +2616,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2133073176"/>
+        <c:axId val="2091996648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2582,13 +2628,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2134940344"/>
+        <c:crossAx val="2091999784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2896,28 +2943,28 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.969015629284343</c:v>
+                  <c:v>0.96857855361596</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.85507149538955</c:v>
+                  <c:v>0.856200527704485</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.461315789473684</c:v>
+                  <c:v>0.449577098243331</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.388420369769705</c:v>
+                  <c:v>0.324910233393178</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.364838306235483</c:v>
+                  <c:v>0.356700655498907</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.29660233445048</c:v>
+                  <c:v>0.288599062133646</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.27884750198626</c:v>
+                  <c:v>0.278769748527625</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.0478306927044952</c:v>
+                  <c:v>0.0474797272392186</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.0379712068847131</c:v>
@@ -3027,8 +3074,8 @@
               <c:idx val="4"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.00490797546012274"/>
-                  <c:y val="-0.0124688279301745"/>
+                  <c:x val="-0.0049079754601227"/>
+                  <c:y val="0.0374062874310287"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -3169,31 +3216,31 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.176103646833013</c:v>
+                  <c:v>0.605187032418953</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0252572497661366</c:v>
+                  <c:v>0.303916122760728</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.212315789473684</c:v>
+                  <c:v>0.219149859032748</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.229646448264677</c:v>
+                  <c:v>0.172172351885099</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.118670716455244</c:v>
+                  <c:v>0.188638018936635</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.1914653877268</c:v>
+                  <c:v>0.195193434935522</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.191195027340281</c:v>
+                  <c:v>0.202580162662429</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.0145081061164333</c:v>
+                  <c:v>0.0142830814596388</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.00611109839555057</c:v>
+                  <c:v>0.00647730653910416</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3210,11 +3257,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2135821608"/>
-        <c:axId val="-2133687080"/>
+        <c:axId val="2091933048"/>
+        <c:axId val="2091930024"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2135821608"/>
+        <c:axId val="2091933048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3234,7 +3281,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133687080"/>
+        <c:crossAx val="2091930024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3242,7 +3289,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2133687080"/>
+        <c:axId val="2091930024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3260,7 +3307,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135821608"/>
+        <c:crossAx val="2091933048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3316,6 +3363,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3563,31 +3611,31 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.941270748738096</c:v>
+                  <c:v>0.979866727707411</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.95323850479656</c:v>
+                  <c:v>0.967402324472764</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.942308299183561</c:v>
+                  <c:v>0.944292097166943</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.959821408107228</c:v>
+                  <c:v>0.961907036999605</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.955264165569284</c:v>
+                  <c:v>0.965822336583178</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.954581244411625</c:v>
+                  <c:v>0.956346765783352</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.972951253764455</c:v>
+                  <c:v>0.974026556375588</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.984144194420638</c:v>
+                  <c:v>0.984150732802721</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.971478791041292</c:v>
+                  <c:v>0.97169228233549</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.960525376543651</c:v>
@@ -3607,11 +3655,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2121138408"/>
-        <c:axId val="2121213160"/>
+        <c:axId val="2094502568"/>
+        <c:axId val="2094505576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2121138408"/>
+        <c:axId val="2094502568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3631,7 +3679,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2121213160"/>
+        <c:crossAx val="2094505576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3639,7 +3687,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2121213160"/>
+        <c:axId val="2094505576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3657,7 +3705,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2121138408"/>
+        <c:crossAx val="2094502568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3934,6 +3982,10 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="summaries_1" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="summaries" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -4261,8 +4313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I2" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4339,7 +4391,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4">
-        <v>12019</v>
+        <v>3958</v>
       </c>
       <c r="C2" s="4">
         <v>0</v>
@@ -4357,7 +4409,7 @@
       </c>
       <c r="G2" s="3">
         <f t="shared" ref="G2:G11" si="2">B2/J2</f>
-        <v>5.8729251261904411E-2</v>
+        <v>2.0133272292588635E-2</v>
       </c>
       <c r="H2" s="3">
         <f t="shared" ref="H2:H11" si="3">C2/J2</f>
@@ -4365,19 +4417,19 @@
       </c>
       <c r="I2" s="3">
         <f t="shared" ref="I2:I11" si="4">D2/J2</f>
-        <v>0.94127074873809558</v>
+        <v>0.97986672770741134</v>
       </c>
       <c r="J2" s="4">
         <f t="shared" ref="J2:J11" si="5">B2+C2+D2</f>
-        <v>204651</v>
+        <v>196590</v>
       </c>
       <c r="K2" s="4">
         <f>B2+C2</f>
-        <v>12019</v>
+        <v>3958</v>
       </c>
       <c r="L2" s="4">
         <f>B2</f>
-        <v>12019</v>
+        <v>3958</v>
       </c>
       <c r="M2" s="3">
         <f>L2/K2</f>
@@ -4393,7 +4445,7 @@
       </c>
       <c r="P2" s="3">
         <f>D2/J2</f>
-        <v>0.94127074873809558</v>
+        <v>0.97986672770741134</v>
       </c>
       <c r="Q2" t="s">
         <v>2</v>
@@ -4404,61 +4456,61 @@
         <v>2</v>
       </c>
       <c r="B3" s="4">
-        <v>2569</v>
+        <v>6067</v>
       </c>
       <c r="C3" s="4">
-        <v>11567</v>
+        <v>3643</v>
       </c>
       <c r="D3" s="4">
         <v>288164</v>
       </c>
       <c r="E3" s="2">
         <f t="shared" si="0"/>
-        <v>0.18173457838143747</v>
+        <v>0.62481977342945416</v>
       </c>
       <c r="F3" s="3">
         <f t="shared" si="1"/>
-        <v>0.81826542161856253</v>
+        <v>0.37518022657054584</v>
       </c>
       <c r="G3" s="3">
         <f t="shared" si="2"/>
-        <v>8.4981806152828309E-3</v>
+        <v>2.0367672237254678E-2</v>
       </c>
       <c r="H3" s="3">
         <f t="shared" si="3"/>
-        <v>3.826331458815746E-2</v>
+        <v>1.223000328998167E-2</v>
       </c>
       <c r="I3" s="3">
         <f t="shared" si="4"/>
-        <v>0.95323850479655969</v>
+        <v>0.96740232447276364</v>
       </c>
       <c r="J3" s="4">
         <f t="shared" si="5"/>
-        <v>302300</v>
+        <v>297874</v>
       </c>
       <c r="K3" s="4">
         <f t="shared" ref="K3:K11" si="6">K2+B3</f>
-        <v>14588</v>
+        <v>10025</v>
       </c>
       <c r="L3" s="4">
         <f t="shared" ref="L3:L11" si="7">B3+C3</f>
-        <v>14136</v>
+        <v>9710</v>
       </c>
       <c r="M3" s="3">
         <f t="shared" ref="M3:M11" si="8">L3/K3</f>
-        <v>0.96901562928434326</v>
+        <v>0.96857855361596013</v>
       </c>
       <c r="N3" s="3">
         <f t="shared" ref="N3:N11" si="9">B3/K3</f>
-        <v>0.17610364683301344</v>
+        <v>0.60518703241895266</v>
       </c>
       <c r="O3" s="3">
         <f t="shared" ref="O3:O11" si="10">C3/K3</f>
-        <v>0.79291198245132988</v>
+        <v>0.36339152119700746</v>
       </c>
       <c r="P3" s="3">
         <f t="shared" ref="P3:P11" si="11">D3/J3</f>
-        <v>0.95323850479655969</v>
+        <v>0.96740232447276364</v>
       </c>
       <c r="Q3" t="s">
         <v>3</v>
@@ -4469,61 +4521,61 @@
         <v>3</v>
       </c>
       <c r="B4" s="4">
-        <v>378</v>
+        <v>4377</v>
       </c>
       <c r="C4" s="4">
-        <v>12419</v>
+        <v>7954</v>
       </c>
       <c r="D4" s="4">
         <v>209020</v>
       </c>
       <c r="E4" s="2">
         <f t="shared" si="0"/>
-        <v>2.9538173009299055E-2</v>
+        <v>0.3549590463060579</v>
       </c>
       <c r="F4" s="3">
         <f t="shared" si="1"/>
-        <v>0.97046182699070094</v>
+        <v>0.6450409536939421</v>
       </c>
       <c r="G4" s="3">
         <f t="shared" si="2"/>
-        <v>1.704107439916688E-3</v>
+        <v>1.9774024061332454E-2</v>
       </c>
       <c r="H4" s="3">
         <f t="shared" si="3"/>
-        <v>5.5987593376522087E-2</v>
+        <v>3.5933878771724548E-2</v>
       </c>
       <c r="I4" s="3">
         <f t="shared" si="4"/>
-        <v>0.94230829918356118</v>
+        <v>0.94429209716694296</v>
       </c>
       <c r="J4" s="4">
         <f t="shared" si="5"/>
-        <v>221817</v>
+        <v>221351</v>
       </c>
       <c r="K4" s="4">
         <f t="shared" si="6"/>
-        <v>14966</v>
+        <v>14402</v>
       </c>
       <c r="L4" s="4">
         <f t="shared" si="7"/>
-        <v>12797</v>
+        <v>12331</v>
       </c>
       <c r="M4" s="3">
         <f t="shared" si="8"/>
-        <v>0.85507149538954963</v>
+        <v>0.85620052770448551</v>
       </c>
       <c r="N4" s="3">
         <f t="shared" si="9"/>
-        <v>2.5257249766136577E-2</v>
+        <v>0.30391612276072766</v>
       </c>
       <c r="O4" s="3">
         <f t="shared" si="10"/>
-        <v>0.8298142456234131</v>
+        <v>0.55228440494375786</v>
       </c>
       <c r="P4" s="3">
         <f t="shared" si="11"/>
-        <v>0.94230829918356118</v>
+        <v>0.94429209716694296</v>
       </c>
       <c r="Q4" t="s">
         <v>4</v>
@@ -4534,61 +4586,61 @@
         <v>4</v>
       </c>
       <c r="B5" s="4">
-        <v>4034</v>
+        <v>4042</v>
       </c>
       <c r="C5" s="4">
-        <v>4731</v>
+        <v>4250</v>
       </c>
       <c r="D5" s="4">
         <v>209386</v>
       </c>
       <c r="E5" s="2">
         <f t="shared" si="0"/>
-        <v>0.46023958927552766</v>
+        <v>0.48745779064158223</v>
       </c>
       <c r="F5" s="3">
         <f t="shared" si="1"/>
-        <v>0.53976041072447234</v>
+        <v>0.51254220935841777</v>
       </c>
       <c r="G5" s="3">
         <f t="shared" si="2"/>
-        <v>1.849177863039821E-2</v>
+        <v>1.8568711583164123E-2</v>
       </c>
       <c r="H5" s="3">
         <f t="shared" si="3"/>
-        <v>2.168681326237331E-2</v>
+        <v>1.9524251417230958E-2</v>
       </c>
       <c r="I5" s="3">
         <f t="shared" si="4"/>
-        <v>0.95982140810722849</v>
+        <v>0.96190703699960489</v>
       </c>
       <c r="J5" s="4">
         <f t="shared" si="5"/>
-        <v>218151</v>
+        <v>217678</v>
       </c>
       <c r="K5" s="4">
         <f t="shared" si="6"/>
-        <v>19000</v>
+        <v>18444</v>
       </c>
       <c r="L5" s="4">
         <f t="shared" si="7"/>
-        <v>8765</v>
+        <v>8292</v>
       </c>
       <c r="M5" s="3">
         <f t="shared" si="8"/>
-        <v>0.46131578947368423</v>
+        <v>0.44957709824333114</v>
       </c>
       <c r="N5" s="3">
         <f t="shared" si="9"/>
-        <v>0.21231578947368421</v>
+        <v>0.21914985903274778</v>
       </c>
       <c r="O5" s="3">
         <f t="shared" si="10"/>
-        <v>0.249</v>
+        <v>0.23042723921058339</v>
       </c>
       <c r="P5" s="3">
         <f t="shared" si="11"/>
-        <v>0.95982140810722849</v>
+        <v>0.96190703699960489</v>
       </c>
       <c r="Q5" s="1" t="s">
         <v>5</v>
@@ -4599,61 +4651,61 @@
         <v>5</v>
       </c>
       <c r="B6" s="4">
-        <v>5664</v>
+        <v>3836</v>
       </c>
       <c r="C6" s="4">
-        <v>3916</v>
+        <v>3403</v>
       </c>
       <c r="D6" s="4">
         <v>204566</v>
       </c>
       <c r="E6" s="2">
         <f t="shared" si="0"/>
-        <v>0.591231732776618</v>
+        <v>0.52990744577980387</v>
       </c>
       <c r="F6" s="3">
         <f t="shared" si="1"/>
-        <v>0.40876826722338205</v>
+        <v>0.47009255422019613</v>
       </c>
       <c r="G6" s="3">
         <f t="shared" si="2"/>
-        <v>2.6449244907679807E-2</v>
+        <v>1.8110998323930028E-2</v>
       </c>
       <c r="H6" s="3">
         <f t="shared" si="3"/>
-        <v>1.8286589523035687E-2</v>
+        <v>1.6066665092892046E-2</v>
       </c>
       <c r="I6" s="3">
         <f t="shared" si="4"/>
-        <v>0.95526416556928451</v>
+        <v>0.96582233658317795</v>
       </c>
       <c r="J6" s="4">
         <f t="shared" si="5"/>
-        <v>214146</v>
+        <v>211805</v>
       </c>
       <c r="K6" s="4">
         <f t="shared" si="6"/>
-        <v>24664</v>
+        <v>22280</v>
       </c>
       <c r="L6" s="4">
         <f t="shared" si="7"/>
-        <v>9580</v>
+        <v>7239</v>
       </c>
       <c r="M6" s="3">
         <f t="shared" si="8"/>
-        <v>0.38842036976970484</v>
+        <v>0.32491023339317776</v>
       </c>
       <c r="N6" s="3">
         <f t="shared" si="9"/>
-        <v>0.22964644826467726</v>
+        <v>0.17217235188509875</v>
       </c>
       <c r="O6" s="3">
         <f t="shared" si="10"/>
-        <v>0.15877392150502756</v>
+        <v>0.15273788150807899</v>
       </c>
       <c r="P6" s="3">
         <f t="shared" si="11"/>
-        <v>0.95526416556928451</v>
+        <v>0.96582233658317795</v>
       </c>
       <c r="Q6" t="s">
         <v>6</v>
@@ -4664,61 +4716,61 @@
         <v>6</v>
       </c>
       <c r="B7" s="4">
-        <v>3321</v>
+        <v>5180</v>
       </c>
       <c r="C7" s="4">
-        <v>6889</v>
+        <v>4615</v>
       </c>
       <c r="D7" s="4">
         <v>214587</v>
       </c>
       <c r="E7" s="2">
         <f t="shared" si="0"/>
-        <v>0.32526934378060723</v>
+        <v>0.52884124553343548</v>
       </c>
       <c r="F7" s="3">
         <f t="shared" si="1"/>
-        <v>0.67473065621939277</v>
+        <v>0.47115875446656458</v>
       </c>
       <c r="G7" s="3">
         <f t="shared" si="2"/>
-        <v>1.4773328825562619E-2</v>
+        <v>2.3085630754695118E-2</v>
       </c>
       <c r="H7" s="3">
         <f t="shared" si="3"/>
-        <v>3.0645426762812671E-2</v>
+        <v>2.0567603461953275E-2</v>
       </c>
       <c r="I7" s="3">
         <f t="shared" si="4"/>
-        <v>0.95458124441162473</v>
+        <v>0.95634676578335165</v>
       </c>
       <c r="J7" s="4">
         <f t="shared" si="5"/>
-        <v>224797</v>
+        <v>224382</v>
       </c>
       <c r="K7" s="4">
         <f t="shared" si="6"/>
-        <v>27985</v>
+        <v>27460</v>
       </c>
       <c r="L7" s="4">
         <f t="shared" si="7"/>
-        <v>10210</v>
+        <v>9795</v>
       </c>
       <c r="M7" s="3">
         <f t="shared" si="8"/>
-        <v>0.3648383062354833</v>
+        <v>0.3567006554989075</v>
       </c>
       <c r="N7" s="3">
         <f t="shared" si="9"/>
-        <v>0.11867071645524388</v>
+        <v>0.18863801893663509</v>
       </c>
       <c r="O7" s="3">
         <f t="shared" si="10"/>
-        <v>0.24616758978023942</v>
+        <v>0.16806263656227238</v>
       </c>
       <c r="P7" s="3">
         <f t="shared" si="11"/>
-        <v>0.95458124441162473</v>
+        <v>0.95634676578335165</v>
       </c>
       <c r="Q7" t="s">
         <v>7</v>
@@ -4729,61 +4781,61 @@
         <v>7</v>
       </c>
       <c r="B8" s="4">
-        <v>6627</v>
+        <v>6660</v>
       </c>
       <c r="C8" s="4">
-        <v>3639</v>
+        <v>3187</v>
       </c>
       <c r="D8" s="4">
         <v>369271</v>
       </c>
       <c r="E8" s="2">
         <f t="shared" si="0"/>
-        <v>0.64552893045002924</v>
+        <v>0.67634812633289332</v>
       </c>
       <c r="F8" s="3">
         <f t="shared" si="1"/>
-        <v>0.35447106954997076</v>
+        <v>0.32365187366710674</v>
       </c>
       <c r="G8" s="3">
         <f t="shared" si="2"/>
-        <v>1.7460748227445547E-2</v>
+        <v>1.7567089929784393E-2</v>
       </c>
       <c r="H8" s="3">
         <f t="shared" si="3"/>
-        <v>9.5879980080993427E-3</v>
+        <v>8.4063536946280583E-3</v>
       </c>
       <c r="I8" s="3">
         <f t="shared" si="4"/>
-        <v>0.97295125376445513</v>
+        <v>0.97402655637558755</v>
       </c>
       <c r="J8" s="4">
         <f t="shared" si="5"/>
-        <v>379537</v>
+        <v>379118</v>
       </c>
       <c r="K8" s="4">
         <f t="shared" si="6"/>
-        <v>34612</v>
+        <v>34120</v>
       </c>
       <c r="L8" s="4">
         <f t="shared" si="7"/>
-        <v>10266</v>
+        <v>9847</v>
       </c>
       <c r="M8" s="3">
         <f t="shared" si="8"/>
-        <v>0.29660233445047962</v>
+        <v>0.28859906213364594</v>
       </c>
       <c r="N8" s="3">
         <f t="shared" si="9"/>
-        <v>0.19146538772679994</v>
+        <v>0.19519343493552169</v>
       </c>
       <c r="O8" s="3">
         <f t="shared" si="10"/>
-        <v>0.10513694672367965</v>
+        <v>9.3405627198124272E-2</v>
       </c>
       <c r="P8" s="3">
         <f t="shared" si="11"/>
-        <v>0.97295125376445513</v>
+        <v>0.97402655637558755</v>
       </c>
       <c r="Q8" t="s">
         <v>8</v>
@@ -4794,61 +4846,61 @@
         <v>8</v>
       </c>
       <c r="B9" s="4">
-        <v>8182</v>
+        <v>8668</v>
       </c>
       <c r="C9" s="4">
-        <v>3751</v>
+        <v>3260</v>
       </c>
       <c r="D9" s="4">
         <v>740662</v>
       </c>
       <c r="E9" s="2">
         <f t="shared" si="0"/>
-        <v>0.68566161065951559</v>
+        <v>0.72669349429912811</v>
       </c>
       <c r="F9" s="3">
         <f t="shared" si="1"/>
-        <v>0.31433838934048436</v>
+        <v>0.27330650570087189</v>
       </c>
       <c r="G9" s="3">
         <f t="shared" si="2"/>
-        <v>1.0871717191849534E-2</v>
+        <v>1.151755936167103E-2</v>
       </c>
       <c r="H9" s="3">
         <f t="shared" si="3"/>
-        <v>4.9840883875125397E-3</v>
+        <v>4.3317078356077017E-3</v>
       </c>
       <c r="I9" s="3">
         <f t="shared" si="4"/>
-        <v>0.98414419442063794</v>
+        <v>0.98415073280272125</v>
       </c>
       <c r="J9" s="4">
         <f t="shared" si="5"/>
-        <v>752595</v>
+        <v>752590</v>
       </c>
       <c r="K9" s="4">
         <f t="shared" si="6"/>
-        <v>42794</v>
+        <v>42788</v>
       </c>
       <c r="L9" s="4">
         <f t="shared" si="7"/>
-        <v>11933</v>
+        <v>11928</v>
       </c>
       <c r="M9" s="3">
         <f t="shared" si="8"/>
-        <v>0.27884750198625974</v>
+        <v>0.27876974852762459</v>
       </c>
       <c r="N9" s="3">
         <f t="shared" si="9"/>
-        <v>0.19119502734028135</v>
+        <v>0.20258016266242873</v>
       </c>
       <c r="O9" s="3">
         <f t="shared" si="10"/>
-        <v>8.7652474645978404E-2</v>
+        <v>7.618958586519585E-2</v>
       </c>
       <c r="P9" s="3">
         <f t="shared" si="11"/>
-        <v>0.98414419442063794</v>
+        <v>0.98415073280272125</v>
       </c>
       <c r="Q9" t="s">
         <v>9</v>
@@ -4859,61 +4911,61 @@
         <v>10</v>
       </c>
       <c r="B10" s="4">
-        <v>630</v>
+        <v>620</v>
       </c>
       <c r="C10" s="4">
-        <v>1447</v>
+        <v>1441</v>
       </c>
       <c r="D10" s="4">
         <v>70746</v>
       </c>
       <c r="E10" s="2">
         <f t="shared" si="0"/>
-        <v>0.30332209918151182</v>
+        <v>0.30082484230955847</v>
       </c>
       <c r="F10" s="3">
         <f t="shared" si="1"/>
-        <v>0.69667790081848824</v>
+        <v>0.69917515769044158</v>
       </c>
       <c r="G10" s="3">
         <f t="shared" si="2"/>
-        <v>8.6511129725498816E-3</v>
+        <v>8.5156647025698071E-3</v>
       </c>
       <c r="H10" s="3">
         <f t="shared" si="3"/>
-        <v>1.9870095986158218E-2</v>
+        <v>1.9792052961940473E-2</v>
       </c>
       <c r="I10" s="3">
         <f t="shared" si="4"/>
-        <v>0.97147879104129187</v>
+        <v>0.97169228233548977</v>
       </c>
       <c r="J10" s="4">
         <f t="shared" si="5"/>
-        <v>72823</v>
+        <v>72807</v>
       </c>
       <c r="K10" s="4">
         <f t="shared" si="6"/>
-        <v>43424</v>
+        <v>43408</v>
       </c>
       <c r="L10" s="4">
         <f t="shared" si="7"/>
-        <v>2077</v>
+        <v>2061</v>
       </c>
       <c r="M10" s="3">
         <f t="shared" si="8"/>
-        <v>4.7830692704495213E-2</v>
+        <v>4.7479727239218575E-2</v>
       </c>
       <c r="N10" s="3">
         <f t="shared" si="9"/>
-        <v>1.4508106116433309E-2</v>
+        <v>1.4283081459638776E-2</v>
       </c>
       <c r="O10" s="3">
         <f t="shared" si="10"/>
-        <v>3.3322586588061899E-2</v>
+        <v>3.31966457795798E-2</v>
       </c>
       <c r="P10" s="3">
         <f t="shared" si="11"/>
-        <v>0.97147879104129187</v>
+        <v>0.97169228233548977</v>
       </c>
       <c r="Q10" t="s">
         <v>11</v>
@@ -4924,29 +4976,29 @@
         <v>15</v>
       </c>
       <c r="B11" s="4">
-        <v>267</v>
+        <v>283</v>
       </c>
       <c r="C11" s="4">
-        <v>1392</v>
+        <v>1376</v>
       </c>
       <c r="D11" s="4">
         <v>40368</v>
       </c>
       <c r="E11" s="2">
         <f t="shared" si="0"/>
-        <v>0.16094032549728751</v>
+        <v>0.17058468957203135</v>
       </c>
       <c r="F11" s="3">
         <f t="shared" si="1"/>
-        <v>0.83905967450271246</v>
+        <v>0.82941531042796868</v>
       </c>
       <c r="G11" s="3">
         <f t="shared" si="2"/>
-        <v>6.353058747947748E-3</v>
+        <v>6.7337663882742049E-3</v>
       </c>
       <c r="H11" s="3">
         <f t="shared" si="3"/>
-        <v>3.3121564708401739E-2</v>
+        <v>3.2740857068075287E-2</v>
       </c>
       <c r="I11" s="3">
         <f t="shared" si="4"/>
@@ -4970,11 +5022,11 @@
       </c>
       <c r="N11" s="3">
         <f t="shared" si="9"/>
-        <v>6.1110983955505712E-3</v>
+        <v>6.4773065391041636E-3</v>
       </c>
       <c r="O11" s="3">
         <f t="shared" si="10"/>
-        <v>3.1860108489162528E-2</v>
+        <v>3.1493900345608936E-2</v>
       </c>
       <c r="P11" s="3">
         <f t="shared" si="11"/>
@@ -4998,203 +5050,206 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A5:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="A2:D11"/>
+      <selection activeCell="A19" sqref="A19:D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1640625" customWidth="1"/>
     <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
+    <row r="5" spans="5:5">
+      <c r="E5" s="1"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B18" t="s">
         <v>25</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C18" t="s">
         <v>26</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D18" t="s">
         <v>27</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E18" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2">
+    <row r="19" spans="1:5">
+      <c r="A19">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>12019</v>
-      </c>
-      <c r="C2">
+      <c r="B19">
+        <v>3958</v>
+      </c>
+      <c r="C19">
         <v>0</v>
       </c>
-      <c r="D2">
+      <c r="D19">
         <v>192632</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E19" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3">
+    <row r="20" spans="1:5">
+      <c r="A20">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>2569</v>
-      </c>
-      <c r="C3">
-        <v>11567</v>
-      </c>
-      <c r="D3">
+      <c r="B20">
+        <v>6067</v>
+      </c>
+      <c r="C20">
+        <v>3643</v>
+      </c>
+      <c r="D20">
         <v>288164</v>
       </c>
-      <c r="F3" t="s">
+      <c r="E20" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4">
+    <row r="21" spans="1:5">
+      <c r="A21">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>378</v>
-      </c>
-      <c r="C4">
-        <v>12419</v>
-      </c>
-      <c r="D4">
+      <c r="B21">
+        <v>4377</v>
+      </c>
+      <c r="C21">
+        <v>7954</v>
+      </c>
+      <c r="D21">
         <v>209020</v>
       </c>
-      <c r="F4" t="s">
+      <c r="E21" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5">
+    <row r="22" spans="1:5">
+      <c r="A22">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>4034</v>
-      </c>
-      <c r="C5">
-        <v>4731</v>
-      </c>
-      <c r="D5">
+      <c r="B22">
+        <v>4042</v>
+      </c>
+      <c r="C22">
+        <v>4250</v>
+      </c>
+      <c r="D22">
         <v>209386</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
-      <c r="A6">
+    <row r="23" spans="1:5">
+      <c r="A23">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>5664</v>
-      </c>
-      <c r="C6">
-        <v>3916</v>
-      </c>
-      <c r="D6">
+      <c r="B23">
+        <v>3836</v>
+      </c>
+      <c r="C23">
+        <v>3403</v>
+      </c>
+      <c r="D23">
         <v>204566</v>
       </c>
-      <c r="F6" t="s">
+      <c r="E23" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
-      <c r="A7">
+    <row r="24" spans="1:5">
+      <c r="A24">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>3321</v>
-      </c>
-      <c r="C7">
-        <v>6889</v>
-      </c>
-      <c r="D7">
+      <c r="B24">
+        <v>5180</v>
+      </c>
+      <c r="C24">
+        <v>4615</v>
+      </c>
+      <c r="D24">
         <v>214587</v>
       </c>
-      <c r="F7" t="s">
+      <c r="E24" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
-      <c r="A8">
+    <row r="25" spans="1:5">
+      <c r="A25">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>6627</v>
-      </c>
-      <c r="C8">
-        <v>3639</v>
-      </c>
-      <c r="D8">
+      <c r="B25">
+        <v>6660</v>
+      </c>
+      <c r="C25">
+        <v>3187</v>
+      </c>
+      <c r="D25">
         <v>369271</v>
       </c>
-      <c r="F8" t="s">
+      <c r="E25" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="A9">
+    <row r="26" spans="1:5">
+      <c r="A26">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>8182</v>
-      </c>
-      <c r="C9">
-        <v>3751</v>
-      </c>
-      <c r="D9">
+      <c r="B26">
+        <v>8668</v>
+      </c>
+      <c r="C26">
+        <v>3260</v>
+      </c>
+      <c r="D26">
         <v>740662</v>
       </c>
-      <c r="F9" t="s">
+      <c r="E26" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
         <v>10</v>
       </c>
-      <c r="B10">
-        <v>630</v>
-      </c>
-      <c r="C10">
-        <v>1447</v>
-      </c>
-      <c r="D10">
+      <c r="B27">
+        <v>620</v>
+      </c>
+      <c r="C27">
+        <v>1441</v>
+      </c>
+      <c r="D27">
         <v>70746</v>
       </c>
-      <c r="F10" t="s">
+      <c r="E27" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11">
+    <row r="28" spans="1:5">
+      <c r="A28">
         <v>9</v>
       </c>
-      <c r="B11">
-        <v>267</v>
-      </c>
-      <c r="C11">
-        <v>1392</v>
-      </c>
-      <c r="D11">
+      <c r="B28">
+        <v>283</v>
+      </c>
+      <c r="C28">
+        <v>1376</v>
+      </c>
+      <c r="D28">
         <v>40368</v>
       </c>
-      <c r="F11" t="s">
+      <c r="E28" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>